<commit_message>
Bang phan chia cong viec_Changed
</commit_message>
<xml_diff>
--- a/congviec.xlsx
+++ b/congviec.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>BẢNG MÔ TẢ CÔNG VIỆC</t>
   </si>
@@ -92,6 +92,30 @@
   </si>
   <si>
     <t>Úp nội dung lên Github</t>
+  </si>
+  <si>
+    <t>Trần Lê Quốc Thịnh</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về ngôn ngữ C#</t>
+  </si>
+  <si>
+    <t>Soạn file word giới thiệu C#</t>
+  </si>
+  <si>
+    <t>Soạn file trình bày chức năng 1</t>
+  </si>
+  <si>
+    <t>Soạn file excel phân chia công việc(5)</t>
+  </si>
+  <si>
+    <t>Code chức năng 1(Login)</t>
+  </si>
+  <si>
+    <t>Code các chức năng khác…</t>
+  </si>
+  <si>
+    <t>4h</t>
   </si>
 </sst>
 </file>
@@ -176,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,6 +220,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -210,13 +244,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -530,34 +557,37 @@
     <col min="2" max="2" width="44.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="18.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -565,10 +595,13 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -581,11 +614,14 @@
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -598,11 +634,14 @@
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -613,9 +652,10 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E6" s="8"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -624,11 +664,12 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -639,9 +680,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E8" s="8"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -652,9 +694,10 @@
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E9" s="8"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -665,22 +708,24 @@
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E10" s="8"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -690,9 +735,10 @@
       <c r="D12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E12" s="8"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -703,9 +749,10 @@
       <c r="D13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E13" s="8"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -716,9 +763,10 @@
       <c r="D14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E14" s="8"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -729,9 +777,10 @@
       <c r="D15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E15" s="8"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -742,11 +791,12 @@
       <c r="D16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E16" s="8"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>24</v>
@@ -755,36 +805,159 @@
       <c r="D17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>14</v>
+      <c r="E17" s="8"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="6" t="s">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="14"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>21</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B30" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new 2 file
</commit_message>
<xml_diff>
--- a/congviec.xlsx
+++ b/congviec.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>BẢNG MÔ TẢ CÔNG VIỆC</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>4h</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về SQL</t>
+  </si>
+  <si>
+    <t>Soạn file word giới thiệu SQL</t>
   </si>
 </sst>
 </file>
@@ -200,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,6 +235,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -545,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -562,32 +571,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -865,30 +874,30 @@
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="8">
+      <c r="A22" s="12">
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="8">
+      <c r="A23" s="12">
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -897,7 +906,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8" t="s">
@@ -911,47 +920,75 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="4"/>
+      <c r="F25" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="4"/>
     </row>
+    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>23</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="4"/>
+    </row>
     <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="11"/>
-    </row>
-    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="11"/>
+      <c r="A28" s="8">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
       <c r="B30" s="10"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B32" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Change file cong viec
</commit_message>
<xml_diff>
--- a/congviec.xlsx
+++ b/congviec.xlsx
@@ -115,13 +115,13 @@
     <t>Code các chức năng khác…</t>
   </si>
   <si>
-    <t>4h</t>
-  </si>
-  <si>
     <t>Tìm hiểu về SQL</t>
   </si>
   <si>
     <t>Soạn file word giới thiệu SQL</t>
+  </si>
+  <si>
+    <t>8h</t>
   </si>
 </sst>
 </file>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -878,7 +878,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -892,7 +892,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -965,7 +965,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>

</xml_diff>

<commit_message>
Chandge file cong viec
</commit_message>
<xml_diff>
--- a/congviec.xlsx
+++ b/congviec.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>BẢNG MÔ TẢ CÔNG VIỆC</t>
   </si>
@@ -121,7 +121,10 @@
     <t>Soạn file word giới thiệu SQL</t>
   </si>
   <si>
-    <t>8h</t>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>12h</t>
   </si>
 </sst>
 </file>
@@ -839,7 +842,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -965,7 +968,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>

</xml_diff>